<commit_message>
methods create_tables() and add_data_to_db_vacancies() have been updated and checked in pgadmin
</commit_message>
<xml_diff>
--- a/src/tables_templates.xlsx
+++ b/src/tables_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_sha\PycharmProjects\Database_Vacancies\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7934BE72-BAF8-4807-8366-F4BB4FDD8FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1A0010-03FF-4A10-B1B1-F855CF2D427F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>company_name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>item['salary']['currency']</t>
   </si>
   <si>
-    <t>item['salary']['gross']</t>
-  </si>
-  <si>
     <t>salary_to</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
   </si>
   <si>
     <t>salary_currency</t>
-  </si>
-  <si>
-    <t>salary_gross</t>
   </si>
   <si>
     <r>
@@ -160,12 +154,15 @@
   <si>
     <t>item['experience']['id']</t>
   </si>
+  <si>
+    <t>item['employer']['alternate_url']</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +181,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,6 +237,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -257,8 +264,8 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -280,8 +287,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2038350" y="723900"/>
-          <a:ext cx="6438900" cy="2352675"/>
+          <a:off x="2314575" y="904875"/>
+          <a:ext cx="7534275" cy="2171700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -572,21 +579,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C06CB9D-BC0C-42BA-857A-130FE0EC62E1}">
   <dimension ref="B3:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.44140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -616,6 +623,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>6</v>
@@ -627,28 +645,28 @@
         <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
@@ -659,66 +677,66 @@
         <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="K19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="H20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
methods get_avg_salary and get_vacancies_with_higher_salary have been added and checked in pgadmin
</commit_message>
<xml_diff>
--- a/src/tables_templates.xlsx
+++ b/src/tables_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_sha\PycharmProjects\Database_Vacancies\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1A0010-03FF-4A10-B1B1-F855CF2D427F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15DDC5-FD95-4649-A48D-3D83A3F02280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>company_name</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>item['employer']['alternate_url']</t>
+  </si>
+  <si>
+    <t>vacancy_link</t>
+  </si>
+  <si>
+    <t>item['alternate_url']</t>
   </si>
 </sst>
 </file>
@@ -577,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C06CB9D-BC0C-42BA-857A-130FE0EC62E1}">
-  <dimension ref="B3:L20"/>
+  <dimension ref="B3:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,12 +599,13 @@
     <col min="6" max="6" width="22.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="19.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -634,7 +641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -657,19 +664,22 @@
         <v>1</v>
       </c>
       <c r="I18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
@@ -695,16 +705,19 @@
         <v>4</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="M19" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="20" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
@@ -727,15 +740,18 @@
         <v>19</v>
       </c>
       <c r="I20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="M20" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>